<commit_message>
Last commit removed all the "containsText" web elements and replaced them with absolute values. This one is one of the last touches. Finished last test case and will add 15-20 more soon hopefully.
</commit_message>
<xml_diff>
--- a/files/Purchase Items.xlsx
+++ b/files/Purchase Items.xlsx
@@ -32,7 +32,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -42,6 +42,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -57,11 +58,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -295,8 +299,8 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>64.99</v>
+      <c r="B2" s="2">
+        <v>64.95</v>
       </c>
     </row>
     <row r="3">

</xml_diff>